<commit_message>
Updating 10 Jan 2018
</commit_message>
<xml_diff>
--- a/TiffinTracker.xlsx
+++ b/TiffinTracker.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SA292082\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SA292082\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -115,7 +115,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="[$-14009]dd\-mm\-yyyy;@"/>
+    <numFmt numFmtId="164" formatCode="[$-14009]dd\-mm\-yyyy;@"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -619,43 +619,13 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
@@ -669,12 +639,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -699,26 +663,62 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
     <xf numFmtId="49" fontId="3" fillId="9" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1044,7 +1044,7 @@
   <dimension ref="B1:L40"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="O4" sqref="O4"/>
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1062,59 +1062,59 @@
   <sheetData>
     <row r="1" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:11" ht="39.75" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="B2" s="56"/>
-      <c r="C2" s="57"/>
-      <c r="D2" s="57"/>
-      <c r="E2" s="59" t="s">
+      <c r="B2" s="44"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="63" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="59"/>
-      <c r="G2" s="59"/>
-      <c r="H2" s="59"/>
-      <c r="I2" s="57"/>
-      <c r="J2" s="57"/>
-      <c r="K2" s="58"/>
+      <c r="F2" s="63"/>
+      <c r="G2" s="63"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="45"/>
+      <c r="J2" s="45"/>
+      <c r="K2" s="46"/>
     </row>
     <row r="3" spans="2:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="51" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="52" t="s">
+      <c r="B3" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="53" t="s">
-        <v>1</v>
-      </c>
-      <c r="E3" s="54" t="s">
+      <c r="D3" s="41" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="54" t="s">
+      <c r="F3" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="54" t="s">
+      <c r="G3" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="54" t="s">
+      <c r="H3" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="54" t="s">
+      <c r="I3" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="J3" s="54" t="s">
+      <c r="J3" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="K3" s="55" t="s">
+      <c r="K3" s="43" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="13">
+      <c r="C4" s="10">
         <v>43101</v>
       </c>
-      <c r="D4" s="27">
+      <c r="D4" s="17">
         <v>0</v>
       </c>
       <c r="E4" s="3">
@@ -1135,18 +1135,18 @@
       <c r="J4" s="3">
         <v>0</v>
       </c>
-      <c r="K4" s="28">
+      <c r="K4" s="18">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="15">
+      <c r="C5" s="12">
         <v>43102</v>
       </c>
-      <c r="D5" s="29">
+      <c r="D5" s="19">
         <v>1</v>
       </c>
       <c r="E5" s="1">
@@ -1172,13 +1172,13 @@
       </c>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="15">
+      <c r="C6" s="12">
         <v>43103</v>
       </c>
-      <c r="D6" s="29">
+      <c r="D6" s="19">
         <v>1</v>
       </c>
       <c r="E6" s="1">
@@ -1204,13 +1204,13 @@
       </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="15">
+      <c r="C7" s="12">
         <v>43104</v>
       </c>
-      <c r="D7" s="29">
+      <c r="D7" s="19">
         <v>1</v>
       </c>
       <c r="E7" s="1">
@@ -1236,13 +1236,13 @@
       </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="15">
+      <c r="C8" s="12">
         <v>43105</v>
       </c>
-      <c r="D8" s="31">
+      <c r="D8" s="21">
         <v>0</v>
       </c>
       <c r="E8" s="2">
@@ -1263,50 +1263,50 @@
       <c r="J8" s="2">
         <v>0</v>
       </c>
-      <c r="K8" s="32">
+      <c r="K8" s="22">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="15">
+      <c r="C9" s="12">
         <v>43106</v>
       </c>
-      <c r="D9" s="60"/>
-      <c r="E9" s="61"/>
-      <c r="F9" s="61"/>
-      <c r="G9" s="61"/>
-      <c r="H9" s="61"/>
-      <c r="I9" s="61"/>
-      <c r="J9" s="61"/>
-      <c r="K9" s="62"/>
+      <c r="D9" s="47"/>
+      <c r="E9" s="48"/>
+      <c r="F9" s="48"/>
+      <c r="G9" s="48"/>
+      <c r="H9" s="48"/>
+      <c r="I9" s="48"/>
+      <c r="J9" s="48"/>
+      <c r="K9" s="49"/>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="15">
+      <c r="C10" s="12">
         <v>43107</v>
       </c>
-      <c r="D10" s="63"/>
-      <c r="E10" s="64"/>
-      <c r="F10" s="64"/>
-      <c r="G10" s="64"/>
-      <c r="H10" s="64"/>
-      <c r="I10" s="64"/>
-      <c r="J10" s="64"/>
-      <c r="K10" s="65"/>
+      <c r="D10" s="50"/>
+      <c r="E10" s="51"/>
+      <c r="F10" s="51"/>
+      <c r="G10" s="51"/>
+      <c r="H10" s="51"/>
+      <c r="I10" s="51"/>
+      <c r="J10" s="51"/>
+      <c r="K10" s="52"/>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="15">
+      <c r="C11" s="12">
         <v>43108</v>
       </c>
-      <c r="D11" s="27">
+      <c r="D11" s="17">
         <v>1</v>
       </c>
       <c r="E11" s="3">
@@ -1327,18 +1327,18 @@
       <c r="J11" s="3">
         <v>0</v>
       </c>
-      <c r="K11" s="28">
+      <c r="K11" s="18">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B12" s="14" t="s">
+      <c r="B12" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="15">
+      <c r="C12" s="12">
         <v>43109</v>
       </c>
-      <c r="D12" s="29">
+      <c r="D12" s="19">
         <v>1</v>
       </c>
       <c r="E12" s="1">
@@ -1359,454 +1359,470 @@
       <c r="J12" s="1">
         <v>1</v>
       </c>
-      <c r="K12" s="30">
+      <c r="K12" s="20">
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B13" s="14" t="s">
+      <c r="B13" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="15">
+      <c r="C13" s="12">
         <v>43110</v>
       </c>
-      <c r="D13" s="29"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-      <c r="K13" s="30"/>
+      <c r="D13" s="19">
+        <v>1</v>
+      </c>
+      <c r="E13" s="1">
+        <v>1</v>
+      </c>
+      <c r="F13" s="1">
+        <v>1</v>
+      </c>
+      <c r="G13" s="1">
+        <v>1</v>
+      </c>
+      <c r="H13" s="1">
+        <v>1</v>
+      </c>
+      <c r="I13" s="1">
+        <v>1</v>
+      </c>
+      <c r="J13" s="1">
+        <v>1</v>
+      </c>
+      <c r="K13" s="20">
+        <v>1</v>
+      </c>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B14" s="14" t="s">
+      <c r="B14" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="15">
+      <c r="C14" s="12">
         <v>43111</v>
       </c>
-      <c r="D14" s="29"/>
+      <c r="D14" s="19"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
-      <c r="K14" s="30"/>
+      <c r="K14" s="20"/>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B15" s="14" t="s">
+      <c r="B15" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="15">
+      <c r="C15" s="12">
         <v>43112</v>
       </c>
-      <c r="D15" s="29"/>
+      <c r="D15" s="19"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
-      <c r="K15" s="30"/>
+      <c r="K15" s="20"/>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B16" s="14" t="s">
+      <c r="B16" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="15">
+      <c r="C16" s="12">
         <v>43113</v>
       </c>
-      <c r="D16" s="33"/>
+      <c r="D16" s="23"/>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
       <c r="J16" s="4"/>
-      <c r="K16" s="34"/>
+      <c r="K16" s="24"/>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B17" s="14" t="s">
+      <c r="B17" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C17" s="15">
+      <c r="C17" s="12">
         <v>43114</v>
       </c>
-      <c r="D17" s="35"/>
+      <c r="D17" s="25"/>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
       <c r="H17" s="5"/>
       <c r="I17" s="5"/>
       <c r="J17" s="5"/>
-      <c r="K17" s="36"/>
+      <c r="K17" s="26"/>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B18" s="14" t="s">
+      <c r="B18" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="15">
+      <c r="C18" s="12">
         <v>43115</v>
       </c>
-      <c r="D18" s="29"/>
+      <c r="D18" s="19"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
-      <c r="K18" s="30"/>
+      <c r="K18" s="20"/>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B19" s="14" t="s">
+      <c r="B19" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C19" s="15">
+      <c r="C19" s="12">
         <v>43116</v>
       </c>
-      <c r="D19" s="29"/>
+      <c r="D19" s="19"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
-      <c r="K19" s="30"/>
+      <c r="K19" s="20"/>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B20" s="14" t="s">
+      <c r="B20" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C20" s="15">
+      <c r="C20" s="12">
         <v>43117</v>
       </c>
-      <c r="D20" s="29"/>
+      <c r="D20" s="19"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
-      <c r="K20" s="30"/>
+      <c r="K20" s="20"/>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B21" s="14" t="s">
+      <c r="B21" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C21" s="15">
+      <c r="C21" s="12">
         <v>43118</v>
       </c>
-      <c r="D21" s="29"/>
+      <c r="D21" s="19"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
-      <c r="K21" s="30"/>
+      <c r="K21" s="20"/>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B22" s="14" t="s">
+      <c r="B22" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C22" s="15">
+      <c r="C22" s="12">
         <v>43119</v>
       </c>
-      <c r="D22" s="29"/>
+      <c r="D22" s="19"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
-      <c r="K22" s="30"/>
+      <c r="K22" s="20"/>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B23" s="14" t="s">
+      <c r="B23" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C23" s="15">
+      <c r="C23" s="12">
         <v>43120</v>
       </c>
-      <c r="D23" s="33"/>
+      <c r="D23" s="23"/>
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
       <c r="H23" s="4"/>
       <c r="I23" s="4"/>
       <c r="J23" s="4"/>
-      <c r="K23" s="34"/>
+      <c r="K23" s="24"/>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B24" s="14" t="s">
+      <c r="B24" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C24" s="15">
+      <c r="C24" s="12">
         <v>43121</v>
       </c>
-      <c r="D24" s="35"/>
+      <c r="D24" s="25"/>
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
       <c r="G24" s="5"/>
       <c r="H24" s="5"/>
       <c r="I24" s="5"/>
       <c r="J24" s="5"/>
-      <c r="K24" s="36"/>
+      <c r="K24" s="26"/>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B25" s="14" t="s">
+      <c r="B25" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C25" s="15">
+      <c r="C25" s="12">
         <v>43122</v>
       </c>
-      <c r="D25" s="29"/>
+      <c r="D25" s="19"/>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
-      <c r="K25" s="30"/>
+      <c r="K25" s="20"/>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B26" s="14" t="s">
+      <c r="B26" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C26" s="15">
+      <c r="C26" s="12">
         <v>43123</v>
       </c>
-      <c r="D26" s="29"/>
+      <c r="D26" s="19"/>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
-      <c r="K26" s="30"/>
+      <c r="K26" s="20"/>
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B27" s="14" t="s">
+      <c r="B27" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C27" s="15">
+      <c r="C27" s="12">
         <v>43124</v>
       </c>
-      <c r="D27" s="29"/>
+      <c r="D27" s="19"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
-      <c r="K27" s="30"/>
+      <c r="K27" s="20"/>
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B28" s="14" t="s">
+      <c r="B28" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C28" s="15">
+      <c r="C28" s="12">
         <v>43125</v>
       </c>
-      <c r="D28" s="29"/>
+      <c r="D28" s="19"/>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
-      <c r="K28" s="30"/>
+      <c r="K28" s="20"/>
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B29" s="14" t="s">
+      <c r="B29" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C29" s="15">
+      <c r="C29" s="12">
         <v>43126</v>
       </c>
-      <c r="D29" s="29"/>
+      <c r="D29" s="19"/>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
-      <c r="K29" s="30"/>
+      <c r="K29" s="20"/>
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B30" s="14" t="s">
+      <c r="B30" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="C30" s="15">
+      <c r="C30" s="12">
         <v>43127</v>
       </c>
-      <c r="D30" s="33"/>
+      <c r="D30" s="23"/>
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
       <c r="G30" s="4"/>
       <c r="H30" s="4"/>
       <c r="I30" s="4"/>
       <c r="J30" s="4"/>
-      <c r="K30" s="34"/>
+      <c r="K30" s="24"/>
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B31" s="14" t="s">
+      <c r="B31" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C31" s="15">
+      <c r="C31" s="12">
         <v>43128</v>
       </c>
-      <c r="D31" s="35"/>
+      <c r="D31" s="25"/>
       <c r="E31" s="5"/>
       <c r="F31" s="5"/>
       <c r="G31" s="5"/>
       <c r="H31" s="5"/>
       <c r="I31" s="5"/>
       <c r="J31" s="5"/>
-      <c r="K31" s="36"/>
+      <c r="K31" s="26"/>
     </row>
     <row r="32" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B32" s="14" t="s">
+      <c r="B32" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C32" s="15">
+      <c r="C32" s="12">
         <v>43129</v>
       </c>
-      <c r="D32" s="29"/>
+      <c r="D32" s="19"/>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
-      <c r="K32" s="30"/>
+      <c r="K32" s="20"/>
     </row>
     <row r="33" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B33" s="14" t="s">
+      <c r="B33" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C33" s="15">
+      <c r="C33" s="12">
         <v>43130</v>
       </c>
-      <c r="D33" s="29"/>
+      <c r="D33" s="19"/>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
-      <c r="K33" s="30"/>
+      <c r="K33" s="20"/>
     </row>
     <row r="34" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="16" t="s">
+      <c r="B34" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C34" s="17">
+      <c r="C34" s="14">
         <v>43131</v>
       </c>
-      <c r="D34" s="37"/>
-      <c r="E34" s="38"/>
-      <c r="F34" s="38"/>
-      <c r="G34" s="38"/>
-      <c r="H34" s="38"/>
-      <c r="I34" s="38"/>
-      <c r="J34" s="38"/>
-      <c r="K34" s="43"/>
-      <c r="L34" s="49" t="s">
+      <c r="D34" s="27"/>
+      <c r="E34" s="28"/>
+      <c r="F34" s="28"/>
+      <c r="G34" s="28"/>
+      <c r="H34" s="28"/>
+      <c r="I34" s="28"/>
+      <c r="J34" s="28"/>
+      <c r="K34" s="31"/>
+      <c r="L34" s="37" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="35" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B35" s="18" t="s">
+      <c r="B35" s="64" t="s">
         <v>24</v>
       </c>
-      <c r="C35" s="19"/>
-      <c r="D35" s="20">
+      <c r="C35" s="65"/>
+      <c r="D35" s="15">
         <f>SUM(D4:D34)</f>
+        <v>6</v>
+      </c>
+      <c r="E35" s="15">
+        <f t="shared" ref="E35:K35" si="0">SUM(E4:E34)</f>
         <v>5</v>
       </c>
-      <c r="E35" s="20">
-        <f t="shared" ref="E35:K35" si="0">SUM(E4:E34)</f>
+      <c r="F35" s="15">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="G35" s="15">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="H35" s="15">
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="F35" s="20">
+      <c r="I35" s="15">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G35" s="20">
+      <c r="J35" s="15">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="H35" s="20">
+      <c r="K35" s="32">
         <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="I35" s="20">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="J35" s="20">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="K35" s="44">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="L35" s="50">
+        <v>2</v>
+      </c>
+      <c r="L35" s="38">
         <f>SUM(D35:K35)</f>
-        <v>25</v>
+        <v>33</v>
       </c>
     </row>
     <row r="36" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B36" s="21" t="s">
+      <c r="B36" s="55" t="s">
         <v>18</v>
       </c>
-      <c r="C36" s="9"/>
+      <c r="C36" s="56"/>
       <c r="D36" s="6">
         <f>30*D35</f>
-        <v>150</v>
+        <v>180</v>
       </c>
       <c r="E36" s="6">
         <f>35*E35</f>
-        <v>140</v>
+        <v>175</v>
       </c>
       <c r="F36" s="6">
         <f>40*F35</f>
-        <v>200</v>
+        <v>240</v>
       </c>
       <c r="G36" s="6">
         <f>40*G35</f>
-        <v>80</v>
+        <v>120</v>
       </c>
       <c r="H36" s="6">
         <f>50*H35</f>
-        <v>150</v>
+        <v>200</v>
       </c>
       <c r="I36" s="6">
         <f>40*I35</f>
-        <v>160</v>
+        <v>200</v>
       </c>
       <c r="J36" s="6">
         <f>40*J35</f>
-        <v>40</v>
-      </c>
-      <c r="K36" s="45">
+        <v>80</v>
+      </c>
+      <c r="K36" s="33">
         <f>35*K35</f>
-        <v>35</v>
-      </c>
-      <c r="L36" s="50">
+        <v>70</v>
+      </c>
+      <c r="L36" s="38">
         <f>SUM(D36:K36)</f>
-        <v>955</v>
+        <v>1265</v>
       </c>
     </row>
     <row r="37" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B37" s="22" t="s">
+      <c r="B37" s="57" t="s">
         <v>20</v>
       </c>
-      <c r="C37" s="10"/>
+      <c r="C37" s="58"/>
       <c r="D37" s="7"/>
       <c r="E37" s="7"/>
       <c r="F37" s="7"/>
@@ -1816,125 +1832,125 @@
       </c>
       <c r="I37" s="7"/>
       <c r="J37" s="7"/>
-      <c r="K37" s="46"/>
-      <c r="L37" s="50">
+      <c r="K37" s="34"/>
+      <c r="L37" s="38">
         <f>SUM(D37:K37)</f>
         <v>250</v>
       </c>
     </row>
     <row r="38" spans="2:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B38" s="23" t="s">
+      <c r="B38" s="59" t="s">
         <v>19</v>
       </c>
-      <c r="C38" s="11"/>
+      <c r="C38" s="60"/>
       <c r="D38" s="8">
         <f>D37-D36</f>
-        <v>-150</v>
+        <v>-180</v>
       </c>
       <c r="E38" s="8">
         <f t="shared" ref="E38:K38" si="1">E37-E36</f>
-        <v>-140</v>
+        <v>-175</v>
       </c>
       <c r="F38" s="8">
         <f t="shared" si="1"/>
-        <v>-200</v>
+        <v>-240</v>
       </c>
       <c r="G38" s="8">
         <f t="shared" si="1"/>
-        <v>-80</v>
+        <v>-120</v>
       </c>
       <c r="H38" s="8">
         <f t="shared" si="1"/>
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="I38" s="8">
         <f t="shared" si="1"/>
-        <v>-160</v>
+        <v>-200</v>
       </c>
       <c r="J38" s="8">
         <f t="shared" si="1"/>
-        <v>-40</v>
-      </c>
-      <c r="K38" s="47">
+        <v>-80</v>
+      </c>
+      <c r="K38" s="35">
         <f t="shared" si="1"/>
-        <v>-35</v>
-      </c>
-      <c r="L38" s="50">
+        <v>-70</v>
+      </c>
+      <c r="L38" s="38">
         <f>SUM(D38:K38)</f>
-        <v>-705</v>
+        <v>-1015</v>
       </c>
     </row>
     <row r="39" spans="2:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B39" s="24" t="s">
+      <c r="B39" s="53" t="s">
         <v>21</v>
       </c>
-      <c r="C39" s="25"/>
-      <c r="D39" s="26">
+      <c r="C39" s="54"/>
+      <c r="D39" s="16">
         <f>D36-D37</f>
-        <v>150</v>
-      </c>
-      <c r="E39" s="26">
+        <v>180</v>
+      </c>
+      <c r="E39" s="16">
         <f t="shared" ref="E39:K39" si="2">E36-E37</f>
-        <v>140</v>
-      </c>
-      <c r="F39" s="26">
+        <v>175</v>
+      </c>
+      <c r="F39" s="16">
+        <f t="shared" si="2"/>
+        <v>240</v>
+      </c>
+      <c r="G39" s="16">
+        <f t="shared" si="2"/>
+        <v>120</v>
+      </c>
+      <c r="H39" s="16">
+        <f t="shared" si="2"/>
+        <v>-50</v>
+      </c>
+      <c r="I39" s="16">
         <f t="shared" si="2"/>
         <v>200</v>
       </c>
-      <c r="G39" s="26">
+      <c r="J39" s="16">
         <f t="shared" si="2"/>
         <v>80</v>
       </c>
-      <c r="H39" s="26">
+      <c r="K39" s="36">
         <f t="shared" si="2"/>
-        <v>-100</v>
-      </c>
-      <c r="I39" s="26">
-        <f t="shared" si="2"/>
-        <v>160</v>
-      </c>
-      <c r="J39" s="26">
-        <f t="shared" si="2"/>
-        <v>40</v>
-      </c>
-      <c r="K39" s="48">
-        <f t="shared" si="2"/>
-        <v>35</v>
-      </c>
-      <c r="L39" s="50">
+        <v>70</v>
+      </c>
+      <c r="L39" s="38">
         <f>SUM(D39:K39)</f>
-        <v>705</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="40" spans="2:12" ht="64.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="39" t="s">
+      <c r="B40" s="61" t="s">
         <v>22</v>
       </c>
-      <c r="C40" s="40"/>
-      <c r="D40" s="41"/>
-      <c r="E40" s="41"/>
-      <c r="F40" s="41"/>
-      <c r="G40" s="41"/>
-      <c r="H40" s="41" t="s">
+      <c r="C40" s="62"/>
+      <c r="D40" s="29"/>
+      <c r="E40" s="29"/>
+      <c r="F40" s="29"/>
+      <c r="G40" s="29"/>
+      <c r="H40" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="I40" s="41"/>
-      <c r="J40" s="41" t="s">
+      <c r="I40" s="29"/>
+      <c r="J40" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="K40" s="42" t="s">
+      <c r="K40" s="30" t="s">
         <v>27</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="E2:H2"/>
+    <mergeCell ref="B35:C35"/>
     <mergeCell ref="B39:C39"/>
     <mergeCell ref="B36:C36"/>
     <mergeCell ref="B37:C37"/>
     <mergeCell ref="B38:C38"/>
     <mergeCell ref="B40:C40"/>
-    <mergeCell ref="E2:H2"/>
-    <mergeCell ref="B35:C35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>